<commit_message>
Upgraded Dijkstra to A* algorithm + improved ending mechanism (single destination)
</commit_message>
<xml_diff>
--- a/timing.xlsx
+++ b/timing.xlsx
@@ -8,24 +8,52 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\FEB-Driververless\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F2300F0-4D6F-4206-B0F1-613299A8EE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C65E9BB4-D90B-49C3-8CEA-3B5A1663E828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="57840" windowHeight="32190"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32190"/>
   </bookViews>
   <sheets>
     <sheet name="timing" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">timing!$A$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">timing!$A$2:$A$101</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">timing!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">timing!$B$2:$B$101</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">timing!$A$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">timing!$A$2:$A$101</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">timing!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">timing!$B$2:$B$101</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Dijkstra (ns)</t>
   </si>
   <si>
     <t xml:space="preserve"> Branch and Bound (ns)</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>Dijkstra (ms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Branch and Bound (ms)</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>Standard deviation</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -569,6 +597,1889 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>timing!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dijkstra (ns)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>timing!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>10132200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6622200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2977000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1971700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1082100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1221600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1075400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1248800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>702100</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>734800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>808900</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>735800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>823000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>709500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1095800</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>993500</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>702000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>647900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1150500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>760100</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1611300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>681700</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>678300</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>667700</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1298300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>764000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>738100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>835800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1905200</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>871900</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>776100</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>765500</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>723600</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>764800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2417700</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>733400</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>777600</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1435700</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>766300</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1016700</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>761700</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>750300</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>932900</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>931700</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>825600</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>798200</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>753900</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>741000</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1218700</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>739600</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>804900</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>690100</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>682200</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1023100</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>871600</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>730300</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1278700</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>660300</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>657400</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>651900</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>667300</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1956900</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>2018900</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>688200</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>669000</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>684100</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>821400</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>759600</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>650900</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>654000</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>642400</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>642400</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>649900</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2772800</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1727600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>659400</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>670800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>806500</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1017600</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>747900</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>692800</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>703100</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>718600</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>680200</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>687700</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>979900</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1335100</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1469900</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>685500</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>658700</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>908500</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>692900</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>885100</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>660800</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2111600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>668000</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>690500</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2401100</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1516300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7562-41DF-B16E-3D316C562BD8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1430912208"/>
+        <c:axId val="1430913168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1430912208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1430913168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1430913168"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="1000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1430912208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{45084C6C-B632-4A02-943C-AA53D5F70171}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>Dijkstra (ns)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{554C0464-F486-44A5-BF77-03498A4C2319}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:v> Branch and Bound (ns)</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:title/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:title/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+        <cx:numFmt formatCode="0,00E+00" sourceLinked="0"/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="t" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AACC5E1E-5D6F-F036-480B-52968E395EB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14478000" y="7453312"/>
+              <a:ext cx="4572000" cy="2743200"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E771EF3-6DE2-E0D3-C457-C4D11F0261B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -886,821 +2797,1671 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>94202600</v>
+        <v>10132200</v>
       </c>
       <c r="B2">
-        <v>699616400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>842579400</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <f>MEDIAN(A:A)/1000000</f>
+        <v>0.76590000000000003</v>
+      </c>
+      <c r="G2">
+        <f>MEDIAN(B:B)/1000000</f>
+        <v>711.69389999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>14744600</v>
+        <v>6622200</v>
       </c>
       <c r="B3">
-        <v>625663900</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>729609800</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGEA(A:A)/1000000</f>
+        <v>1.207760696517413</v>
+      </c>
+      <c r="G3">
+        <f>AVERAGEA(B:B)/1000000</f>
+        <v>715.12196865671649</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>13546300</v>
+        <v>2977000</v>
       </c>
       <c r="B4">
-        <v>617029400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>694222800</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <f>_xlfn.STDEV.S(A:A)/1000000</f>
+        <v>1.3951569861235678</v>
+      </c>
+      <c r="G4">
+        <f>_xlfn.STDEV.S(B:B)/1000000</f>
+        <v>31.071275806293215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8678300</v>
+        <v>1971700</v>
       </c>
       <c r="B5">
-        <v>628203700</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>706362900</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5713400</v>
+        <v>1082100</v>
       </c>
       <c r="B6">
-        <v>619928700</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>724411900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3629100</v>
+        <v>1221600</v>
       </c>
       <c r="B7">
-        <v>611405900</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>707009400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5746700</v>
+        <v>1075400</v>
       </c>
       <c r="B8">
-        <v>612335200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>751854000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3126800</v>
+        <v>1248800</v>
       </c>
       <c r="B9">
-        <v>613536300</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>703337900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2734100</v>
+        <v>702100</v>
       </c>
       <c r="B10">
-        <v>605525700</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>680645600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2897800</v>
+        <v>734800</v>
       </c>
       <c r="B11">
-        <v>620021400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>701023100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2702400</v>
+        <v>808900</v>
       </c>
       <c r="B12">
-        <v>627683100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>702577000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2688900</v>
+        <v>735800</v>
       </c>
       <c r="B13">
-        <v>609869000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>747859700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2991900</v>
+        <v>823000</v>
       </c>
       <c r="B14">
-        <v>608896000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>709239000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3122200</v>
+        <v>709500</v>
       </c>
       <c r="B15">
-        <v>631948900</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>690529300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3669600</v>
+        <v>1095800</v>
       </c>
       <c r="B16">
-        <v>612603500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>705169100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2076700</v>
+        <v>993500</v>
       </c>
       <c r="B17">
-        <v>608744800</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>730788300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2073600</v>
+        <v>702000</v>
       </c>
       <c r="B18">
-        <v>609860400</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>695716700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2003800</v>
+        <v>647900</v>
       </c>
       <c r="B19">
-        <v>614475200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>707445800</v>
+      </c>
+      <c r="G19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2454100</v>
+        <v>1150500</v>
       </c>
       <c r="B20">
-        <v>622727200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>726982500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2122100</v>
+        <v>760100</v>
       </c>
       <c r="B21">
-        <v>679542700</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>705840000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2725200</v>
+        <v>1611300</v>
       </c>
       <c r="B22">
-        <v>620790800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>723152200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2123100</v>
+        <v>681700</v>
       </c>
       <c r="B23">
-        <v>609361100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>694505200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1987200</v>
+        <v>678300</v>
       </c>
       <c r="B24">
-        <v>613093300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>682443900</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1998200</v>
+        <v>667700</v>
       </c>
       <c r="B25">
-        <v>618799600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>735303800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1957700</v>
+        <v>1298300</v>
       </c>
       <c r="B26">
-        <v>609807200</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>712113300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2579300</v>
+        <v>764000</v>
       </c>
       <c r="B27">
-        <v>606994800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>701675700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2815900</v>
+        <v>738100</v>
       </c>
       <c r="B28">
-        <v>619270500</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>723983400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2845500</v>
+        <v>835800</v>
       </c>
       <c r="B29">
-        <v>605909600</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>729178100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2611500</v>
+        <v>1905200</v>
       </c>
       <c r="B30">
-        <v>623726400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>711478200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2948200</v>
+        <v>871900</v>
       </c>
       <c r="B31">
-        <v>604576900</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>752969900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2781800</v>
+        <v>776100</v>
       </c>
       <c r="B32">
-        <v>608648500</v>
+        <v>749410900</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2789700</v>
+        <v>765500</v>
       </c>
       <c r="B33">
-        <v>606992500</v>
+        <v>709589900</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3078200</v>
+        <v>723600</v>
       </c>
       <c r="B34">
-        <v>606470700</v>
+        <v>712512300</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2745000</v>
+        <v>764800</v>
       </c>
       <c r="B35">
-        <v>617507200</v>
+        <v>689177300</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>2865700</v>
+        <v>2417700</v>
       </c>
       <c r="B36">
-        <v>611292000</v>
+        <v>716488500</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2683200</v>
+        <v>733400</v>
       </c>
       <c r="B37">
-        <v>606564200</v>
+        <v>699215800</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2702000</v>
+        <v>777600</v>
       </c>
       <c r="B38">
-        <v>605278200</v>
+        <v>700275700</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2733700</v>
+        <v>1435700</v>
       </c>
       <c r="B39">
-        <v>609411700</v>
+        <v>735686100</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2796200</v>
+        <v>766300</v>
       </c>
       <c r="B40">
-        <v>612617800</v>
+        <v>700348000</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>2783400</v>
+        <v>1016700</v>
       </c>
       <c r="B41">
-        <v>609249900</v>
+        <v>699413500</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>3196300</v>
+        <v>761700</v>
       </c>
       <c r="B42">
-        <v>606743100</v>
+        <v>683785000</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2721900</v>
+        <v>750300</v>
       </c>
       <c r="B43">
-        <v>604912100</v>
+        <v>701371600</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>2795700</v>
+        <v>932900</v>
       </c>
       <c r="B44">
-        <v>608094500</v>
+        <v>698845800</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>2694300</v>
+        <v>931700</v>
       </c>
       <c r="B45">
-        <v>614356900</v>
+        <v>723279000</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2970100</v>
+        <v>825600</v>
       </c>
       <c r="B46">
-        <v>608075500</v>
+        <v>679056800</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2585300</v>
+        <v>798200</v>
       </c>
       <c r="B47">
-        <v>607213000</v>
+        <v>702680500</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>2895600</v>
+        <v>753900</v>
       </c>
       <c r="B48">
-        <v>610610400</v>
+        <v>694955600</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>2707400</v>
+        <v>741000</v>
       </c>
       <c r="B49">
-        <v>609704500</v>
+        <v>694667700</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>3243700</v>
+        <v>750000</v>
       </c>
       <c r="B50">
-        <v>618145700</v>
+        <v>733498400</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2943100</v>
+        <v>1218700</v>
       </c>
       <c r="B51">
-        <v>606816600</v>
+        <v>701380400</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>2660100</v>
+        <v>739600</v>
       </c>
       <c r="B52">
-        <v>606883200</v>
+        <v>692671400</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>2818200</v>
+        <v>804900</v>
       </c>
       <c r="B53">
-        <v>607058800</v>
+        <v>712017700</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>2785700</v>
+        <v>690100</v>
       </c>
       <c r="B54">
-        <v>612859700</v>
+        <v>697385500</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1869800</v>
+        <v>682200</v>
       </c>
       <c r="B55">
-        <v>614074600</v>
+        <v>683662000</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1868200</v>
+        <v>1023100</v>
       </c>
       <c r="B56">
-        <v>607613300</v>
+        <v>713881100</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1999700</v>
+        <v>871600</v>
       </c>
       <c r="B57">
-        <v>608735200</v>
+        <v>696974000</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2709300</v>
+        <v>730300</v>
       </c>
       <c r="B58">
-        <v>605930600</v>
+        <v>694607500</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2369200</v>
+        <v>1278700</v>
       </c>
       <c r="B59">
-        <v>639885500</v>
+        <v>742210700</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>2845700</v>
+        <v>660300</v>
       </c>
       <c r="B60">
-        <v>608690300</v>
+        <v>690010000</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1895300</v>
+        <v>657400</v>
       </c>
       <c r="B61">
-        <v>608964300</v>
+        <v>711909600</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2083900</v>
+        <v>651900</v>
       </c>
       <c r="B62">
-        <v>610096400</v>
+        <v>697362300</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>1876700</v>
+        <v>667300</v>
       </c>
       <c r="B63">
-        <v>604873800</v>
+        <v>686843000</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>1871800</v>
+        <v>1956900</v>
       </c>
       <c r="B64">
-        <v>613822700</v>
+        <v>708222700</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1896000</v>
+        <v>2018900</v>
       </c>
       <c r="B65">
-        <v>609433300</v>
+        <v>730280200</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>2005600</v>
+        <v>688200</v>
       </c>
       <c r="B66">
-        <v>606324400</v>
+        <v>698209600</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1908600</v>
+        <v>669000</v>
       </c>
       <c r="B67">
-        <v>608715600</v>
+        <v>719227000</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>1947000</v>
+        <v>684100</v>
       </c>
       <c r="B68">
-        <v>604839000</v>
+        <v>723645800</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>1966100</v>
+        <v>821400</v>
       </c>
       <c r="B69">
-        <v>619464200</v>
+        <v>675518000</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>2080700</v>
+        <v>759600</v>
       </c>
       <c r="B70">
-        <v>607748000</v>
+        <v>720816000</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1866400</v>
+        <v>650900</v>
       </c>
       <c r="B71">
-        <v>609967300</v>
+        <v>729344400</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>1904700</v>
+        <v>654000</v>
       </c>
       <c r="B72">
-        <v>607286000</v>
+        <v>694971900</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>2133300</v>
+        <v>642400</v>
       </c>
       <c r="B73">
-        <v>605228000</v>
+        <v>701231000</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>2337900</v>
+        <v>642400</v>
       </c>
       <c r="B74">
-        <v>613952700</v>
+        <v>695511200</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>1959900</v>
+        <v>649900</v>
       </c>
       <c r="B75">
-        <v>604725500</v>
+        <v>683017100</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>1817700</v>
+        <v>2772800</v>
       </c>
       <c r="B76">
-        <v>604901300</v>
+        <v>726457200</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>2211100</v>
+        <v>1727600</v>
       </c>
       <c r="B77">
-        <v>606134900</v>
+        <v>683339200</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1911900</v>
+        <v>659400</v>
       </c>
       <c r="B78">
-        <v>606341500</v>
+        <v>700627900</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>1981800</v>
+        <v>670800</v>
       </c>
       <c r="B79">
-        <v>619950300</v>
+        <v>711300300</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>1940300</v>
+        <v>806500</v>
       </c>
       <c r="B80">
-        <v>606533600</v>
+        <v>691572900</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>1833100</v>
+        <v>1017600</v>
       </c>
       <c r="B81">
-        <v>605971400</v>
+        <v>706413700</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>1891600</v>
+        <v>747900</v>
       </c>
       <c r="B82">
-        <v>608847000</v>
+        <v>725211600</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1877500</v>
+        <v>692800</v>
       </c>
       <c r="B83">
-        <v>606028800</v>
+        <v>696494700</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>1869500</v>
+        <v>703100</v>
       </c>
       <c r="B84">
-        <v>621223600</v>
+        <v>725323900</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>1844400</v>
+        <v>718600</v>
       </c>
       <c r="B85">
-        <v>605815200</v>
+        <v>729252300</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1845400</v>
+        <v>680200</v>
       </c>
       <c r="B86">
-        <v>606078100</v>
+        <v>696741000</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>2027700</v>
+        <v>687700</v>
       </c>
       <c r="B87">
-        <v>606608000</v>
+        <v>706812000</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>1990100</v>
+        <v>979900</v>
       </c>
       <c r="B88">
-        <v>603148700</v>
+        <v>696881700</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>1876700</v>
+        <v>1335100</v>
       </c>
       <c r="B89">
-        <v>620346900</v>
+        <v>690892600</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>1830100</v>
+        <v>1469900</v>
       </c>
       <c r="B90">
-        <v>606647100</v>
+        <v>714145400</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1804500</v>
+        <v>685500</v>
       </c>
       <c r="B91">
-        <v>606899900</v>
+        <v>698908300</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>1825300</v>
+        <v>658700</v>
       </c>
       <c r="B92">
-        <v>604825700</v>
+        <v>700553900</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>1827200</v>
+        <v>908500</v>
       </c>
       <c r="B93">
-        <v>606415100</v>
+        <v>693973900</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>2193000</v>
+        <v>692900</v>
       </c>
       <c r="B94">
-        <v>624430700</v>
+        <v>681417800</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>2012100</v>
+        <v>885100</v>
       </c>
       <c r="B95">
-        <v>610794900</v>
+        <v>692744400</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>2056900</v>
+        <v>660800</v>
       </c>
       <c r="B96">
-        <v>610216600</v>
+        <v>688352600</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1833400</v>
+        <v>2111600</v>
       </c>
       <c r="B97">
-        <v>606864700</v>
+        <v>716293600</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>2429200</v>
+        <v>668000</v>
       </c>
       <c r="B98">
-        <v>607410700</v>
+        <v>716221200</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1920700</v>
+        <v>690500</v>
       </c>
       <c r="B99">
-        <v>643689700</v>
+        <v>688173900</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>1919400</v>
+        <v>2401100</v>
       </c>
       <c r="B100">
-        <v>609733500</v>
+        <v>692160000</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>1852200</v>
+        <v>1516300</v>
       </c>
       <c r="B101">
-        <v>604691000</v>
+        <v>736640900</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>14357700</v>
+      </c>
+      <c r="B102">
+        <v>850987600</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>4856800</v>
+      </c>
+      <c r="B103">
+        <v>727891500</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>3521900</v>
+      </c>
+      <c r="B104">
+        <v>754968100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>4719000</v>
+      </c>
+      <c r="B105">
+        <v>724845000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>1363000</v>
+      </c>
+      <c r="B106">
+        <v>695823000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>1081200</v>
+      </c>
+      <c r="B107">
+        <v>747643900</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>879300</v>
+      </c>
+      <c r="B108">
+        <v>723497800</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>1544500</v>
+      </c>
+      <c r="B109">
+        <v>727899700</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>1245500</v>
+      </c>
+      <c r="B110">
+        <v>719020800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>679900</v>
+      </c>
+      <c r="B111">
+        <v>687380700</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>1008100</v>
+      </c>
+      <c r="B112">
+        <v>702774900</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>732600</v>
+      </c>
+      <c r="B113">
+        <v>734101600</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>719900</v>
+      </c>
+      <c r="B114">
+        <v>696748200</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>934800</v>
+      </c>
+      <c r="B115">
+        <v>705510900</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>785800</v>
+      </c>
+      <c r="B116">
+        <v>706538800</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>648600</v>
+      </c>
+      <c r="B117">
+        <v>700194700</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>646800</v>
+      </c>
+      <c r="B118">
+        <v>716493400</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>1996600</v>
+      </c>
+      <c r="B119">
+        <v>723823500</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>655400</v>
+      </c>
+      <c r="B120">
+        <v>729911100</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>1780600</v>
+      </c>
+      <c r="B121">
+        <v>705473400</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>652100</v>
+      </c>
+      <c r="B122">
+        <v>691990600</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>712300</v>
+      </c>
+      <c r="B123">
+        <v>703339400</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>656900</v>
+      </c>
+      <c r="B124">
+        <v>707732000</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>647900</v>
+      </c>
+      <c r="B125">
+        <v>745241500</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>772700</v>
+      </c>
+      <c r="B126">
+        <v>786530400</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2554800</v>
+      </c>
+      <c r="B127">
+        <v>783196400</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>756600</v>
+      </c>
+      <c r="B128">
+        <v>757616900</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>1255200</v>
+      </c>
+      <c r="B129">
+        <v>716526700</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>707700</v>
+      </c>
+      <c r="B130">
+        <v>805651300</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>749500</v>
+      </c>
+      <c r="B131">
+        <v>782028100</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>726100</v>
+      </c>
+      <c r="B132">
+        <v>782895900</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>723600</v>
+      </c>
+      <c r="B133">
+        <v>751955800</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>733600</v>
+      </c>
+      <c r="B134">
+        <v>812373700</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>1281200</v>
+      </c>
+      <c r="B135">
+        <v>940991200</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>786700</v>
+      </c>
+      <c r="B136">
+        <v>753652900</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>2873300</v>
+      </c>
+      <c r="B137">
+        <v>707345900</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>902700</v>
+      </c>
+      <c r="B138">
+        <v>715869100</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>728500</v>
+      </c>
+      <c r="B139">
+        <v>734501500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>956000</v>
+      </c>
+      <c r="B140">
+        <v>707517900</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>723700</v>
+      </c>
+      <c r="B141">
+        <v>731137600</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>972200</v>
+      </c>
+      <c r="B142">
+        <v>733851100</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>716200</v>
+      </c>
+      <c r="B143">
+        <v>704240700</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>1299200</v>
+      </c>
+      <c r="B144">
+        <v>738360600</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>726700</v>
+      </c>
+      <c r="B145">
+        <v>726157400</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>1318900</v>
+      </c>
+      <c r="B146">
+        <v>698945100</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>953800</v>
+      </c>
+      <c r="B147">
+        <v>728951600</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>834100</v>
+      </c>
+      <c r="B148">
+        <v>732228200</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>747100</v>
+      </c>
+      <c r="B149">
+        <v>713724900</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>774200</v>
+      </c>
+      <c r="B150">
+        <v>714484800</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>735100</v>
+      </c>
+      <c r="B151">
+        <v>712378300</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>803900</v>
+      </c>
+      <c r="B152">
+        <v>707551700</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>1208100</v>
+      </c>
+      <c r="B153">
+        <v>739330700</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1729200</v>
+      </c>
+      <c r="B154">
+        <v>707733100</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>694900</v>
+      </c>
+      <c r="B155">
+        <v>708402000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>1084600</v>
+      </c>
+      <c r="B156">
+        <v>726501800</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>665800</v>
+      </c>
+      <c r="B157">
+        <v>690823000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>2687800</v>
+      </c>
+      <c r="B158">
+        <v>723256000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>684500</v>
+      </c>
+      <c r="B159">
+        <v>720082300</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>660400</v>
+      </c>
+      <c r="B160">
+        <v>767090700</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>721600</v>
+      </c>
+      <c r="B161">
+        <v>738917100</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1353000</v>
+      </c>
+      <c r="B162">
+        <v>722944200</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>653000</v>
+      </c>
+      <c r="B163">
+        <v>723386500</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>747500</v>
+      </c>
+      <c r="B164">
+        <v>762363800</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>717400</v>
+      </c>
+      <c r="B165">
+        <v>707653600</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>685800</v>
+      </c>
+      <c r="B166">
+        <v>741568800</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>1159100</v>
+      </c>
+      <c r="B167">
+        <v>733620300</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>667300</v>
+      </c>
+      <c r="B168">
+        <v>705284800</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>643700</v>
+      </c>
+      <c r="B169">
+        <v>741580600</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>642800</v>
+      </c>
+      <c r="B170">
+        <v>726039900</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>794500</v>
+      </c>
+      <c r="B171">
+        <v>722608600</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>3414800</v>
+      </c>
+      <c r="B172">
+        <v>736272500</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>921100</v>
+      </c>
+      <c r="B173">
+        <v>717520700</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>637400</v>
+      </c>
+      <c r="B174">
+        <v>703191600</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>738600</v>
+      </c>
+      <c r="B175">
+        <v>724083800</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1081700</v>
+      </c>
+      <c r="B176">
+        <v>710462400</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>1298700</v>
+      </c>
+      <c r="B177">
+        <v>721114700</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>675300</v>
+      </c>
+      <c r="B178">
+        <v>709097400</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>693600</v>
+      </c>
+      <c r="B179">
+        <v>723875500</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>2975500</v>
+      </c>
+      <c r="B180">
+        <v>706844000</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>855700</v>
+      </c>
+      <c r="B181">
+        <v>747982900</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>876900</v>
+      </c>
+      <c r="B182">
+        <v>703731700</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>823900</v>
+      </c>
+      <c r="B183">
+        <v>703854800</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>660300</v>
+      </c>
+      <c r="B184">
+        <v>702990800</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>1183400</v>
+      </c>
+      <c r="B185">
+        <v>687401600</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>664400</v>
+      </c>
+      <c r="B186">
+        <v>727447100</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>676600</v>
+      </c>
+      <c r="B187">
+        <v>739259800</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>715800</v>
+      </c>
+      <c r="B188">
+        <v>699620800</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>667400</v>
+      </c>
+      <c r="B189">
+        <v>737337000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>1352000</v>
+      </c>
+      <c r="B190">
+        <v>713540600</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>686100</v>
+      </c>
+      <c r="B191">
+        <v>722322300</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>1518900</v>
+      </c>
+      <c r="B192">
+        <v>755121900</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>652400</v>
+      </c>
+      <c r="B193">
+        <v>701399800</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>2983500</v>
+      </c>
+      <c r="B194">
+        <v>727034200</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>2647700</v>
+      </c>
+      <c r="B195">
+        <v>710510700</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>682100</v>
+      </c>
+      <c r="B196">
+        <v>701416500</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>1059200</v>
+      </c>
+      <c r="B197">
+        <v>711204600</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>1110800</v>
+      </c>
+      <c r="B198">
+        <v>705272700</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>703000</v>
+      </c>
+      <c r="B199">
+        <v>697130600</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>4287600</v>
+      </c>
+      <c r="B200">
+        <v>780251300</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>641400</v>
+      </c>
+      <c r="B201">
+        <v>730452500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>